<commit_message>
Added sources, updated diary
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4f02f64fd1b16aca/Documents/EPQ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hrsfc-my.sharepoint.com/personal/oc154750_hrsfc_ac_uk/Documents/Documents/EPQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="11_AD4DB114E441178AC67DF49DDE90F218683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E2F88D1-06D8-4856-9489-D3E30976DC96}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="11_AD4DB114E441178AC67DF49DDE90F218683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB4472A4-5C23-44BB-9DD3-54F6ACD34ADF}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>Week Beginning</t>
   </si>
@@ -81,13 +81,19 @@
  - Confirmed project idea - writing a piece of music</t>
   </si>
   <si>
-    <t>Continued setup - added to a Git repository on GitHub so that collaboration between home and school account is easy (Onedrive was being bad at its job)</t>
-  </si>
-  <si>
     <t>Using my school and home GitHub accounts instead.</t>
   </si>
   <si>
     <t>Onedrive not working for sharing between school and home accounts.</t>
+  </si>
+  <si>
+    <t>Continued setup - added to a Git repository on GitHub so that collaboration between home and school account is easy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Set up a GitHub repo that is accessible by both home and school accounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPQ Session was cancelled, week was busy. Did some listening. (R) </t>
   </si>
 </sst>
 </file>
@@ -425,9 +431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,15 +527,19 @@
         <v>2</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -538,6 +548,12 @@
     <row r="5" spans="1:10" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45250</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>

</xml_diff>

<commit_message>
Added timeline document. Updated .md
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hrsfc-my.sharepoint.com/personal/oc154750_hrsfc_ac_uk/Documents/Documents/EPQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="11_AD4DB114E441178AC67DF49DDE90F218683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB4472A4-5C23-44BB-9DD3-54F6ACD34ADF}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="11_AD4DB114E441178AC67DF49DDE90F218683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66209430-EC16-434B-AD6A-26A799EC8A6F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Week Beginning</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t xml:space="preserve">EPQ Session was cancelled, week was busy. Did some listening. (R) </t>
+  </si>
+  <si>
+    <t>Format &amp; General research</t>
   </si>
 </sst>
 </file>
@@ -129,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -149,6 +152,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,6 +170,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,8 +442,8 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,6 +589,9 @@
       <c r="A7" s="2">
         <v>45264</v>
       </c>
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>

</xml_diff>

<commit_message>
Started working on evaluation of project ideas.
Partial diary update as well.
</commit_message>
<xml_diff>
--- a/Diary.xlsx
+++ b/Diary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hrsfc-my.sharepoint.com/personal/oc154750_hrsfc_ac_uk/Documents/Documents/EPQ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hrsfc-my.sharepoint.com/personal/oc154750_hrsfc_ac_uk/Documents/Documents/Subjects/EPQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="11_AD4DB114E441178AC67DF49DDE90F218683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F546BAFF-5D71-474D-B39D-372A3F425E8C}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="11_AD4DB114E441178AC67DF49DDE90F218683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7B2D29C-E3F3-45C3-B4E3-2650E3B95152}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Week Beginning</t>
   </si>
@@ -122,6 +122,12 @@
   </si>
   <si>
     <t>Updated diary, tidied research. Am leaving session early</t>
+  </si>
+  <si>
+    <t>Literally Christmas. Did nothing.</t>
+  </si>
+  <si>
+    <t>Evaluation of project idea shortlist. Further research, and evaluation of research.</t>
   </si>
 </sst>
 </file>
@@ -467,8 +473,8 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -668,6 +674,9 @@
       <c r="A9" s="2">
         <v>45278</v>
       </c>
+      <c r="B9" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -680,6 +689,12 @@
       <c r="A10" s="2">
         <v>45285</v>
       </c>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -692,6 +707,9 @@
       <c r="A11" s="2">
         <v>45292</v>
       </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -703,6 +721,12 @@
     <row r="12" spans="1:10" ht="71.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45299</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>

</xml_diff>